<commit_message>
Import data from excel
</commit_message>
<xml_diff>
--- a/src/server/excel_files/excel.xlsx
+++ b/src/server/excel_files/excel.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hien.phan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhvu/Projects/teachingaids/src/server/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="10665" activeTab="1"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="32000" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Tranh" sheetId="1" r:id="rId1"/>
     <sheet name="Thiết bị" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,18 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>TÊN TRANH</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lớp </t>
-  </si>
-  <si>
-    <t>Mã KH</t>
   </si>
   <si>
     <t>Đ.vị tính</t>
@@ -306,6 +306,54 @@
   <si>
     <t>Mã 
 KH</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>khCode</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>totalNumber</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>8,10</t>
+  </si>
+  <si>
+    <t>8,11</t>
+  </si>
+  <si>
+    <t>8,12</t>
+  </si>
+  <si>
+    <t>8,13</t>
+  </si>
+  <si>
+    <t>8,14</t>
+  </si>
+  <si>
+    <t>8,15</t>
+  </si>
+  <si>
+    <t>8,16</t>
+  </si>
+  <si>
+    <t>8,17</t>
+  </si>
+  <si>
+    <t>8,18</t>
   </si>
 </sst>
 </file>
@@ -365,53 +413,53 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,804 +784,808 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="9">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="9">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="9">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="9">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="9">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="9">
         <v>9</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F12" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="9">
         <v>8</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="9">
         <v>8</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="9">
         <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F15" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="9">
         <v>8</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9">
         <v>9</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F17" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="9">
         <v>8</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="9">
         <v>7</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F19" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="9">
         <v>7</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F20" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="9">
         <v>8</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F21" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="9">
         <v>7</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F22" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9">
         <v>8</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F23" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="9">
         <v>9</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="9">
         <v>8</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F25" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="9">
         <v>7</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F26" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="9">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F27" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="9">
         <v>8</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F28" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="9">
         <v>9</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F29" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="9">
         <v>9</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F30" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="9">
         <v>9</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F31" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="9">
         <v>9</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F32" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" s="9">
         <v>9</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F33" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="9">
         <v>7</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F34" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="9">
         <v>8</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F35" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F36" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="9">
         <v>9</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F37" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C38" s="9">
         <v>9</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F38" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" s="9">
         <v>9</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F39" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="9">
         <v>9</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F40" s="9">
         <v>1</v>
@@ -1548,61 +1600,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="5" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="37" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="6">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="6">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="F2" s="6">
         <v>8</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel template: add category column
</commit_message>
<xml_diff>
--- a/src/server/excel_files/excel.xlsx
+++ b/src/server/excel_files/excel.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="110">
   <si>
     <t>STT</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -782,10 +785,12 @@
     <col min="3" max="5" width="8.83203125" style="8"/>
     <col min="6" max="6" width="14.33203125" style="8" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="8"/>
+    <col min="8" max="8" width="8.83203125" style="8"/>
+    <col min="9" max="9" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -810,8 +815,11 @@
       <c r="H1" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -833,7 +841,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -855,7 +863,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -877,7 +885,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -899,7 +907,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -921,7 +929,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -943,7 +951,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -965,7 +973,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -987,7 +995,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1009,7 +1017,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1031,7 +1039,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1053,7 +1061,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1075,7 +1083,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1097,7 +1105,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1119,7 +1127,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>

</xml_diff>